<commit_message>
Extended loading all country=specific parameters from the country-specific folders.
</commit_message>
<xml_diff>
--- a/input/EL/parameters.xlsx
+++ b/input/EL/parameters.xlsx
@@ -1,42 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsEU\input\EL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4732A4-E8D2-43F2-A798-9CBB828AAA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9798C423-3424-C748-BB9F-B8CAF277D90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
   <si>
     <t>MIN_AGE_TO_HAVE_INCOME</t>
   </si>
   <si>
-    <t>KEY</t>
-  </si>
-  <si>
-    <t>VALUE</t>
-  </si>
-  <si>
     <t>MAX_LABOUR_HOURS_IN_WEEK</t>
+  </si>
+  <si>
+    <t>HOURS_IN_WEEK</t>
+  </si>
+  <si>
+    <t>USE_CONTINUOUS_LABOUR_SUPPLY_HOURS</t>
+  </si>
+  <si>
+    <t>AGE_TO_BECOME_RESPONSIBLE</t>
+  </si>
+  <si>
+    <t>MIN_AGE_TO_LEAVE_EDUCATION</t>
+  </si>
+  <si>
+    <t>MAX_AGE_TO_LEAVE_CONTINUOUS_EDUCATION</t>
+  </si>
+  <si>
+    <t>MAX_AGE_TO_ENTER_EDUCATION</t>
+  </si>
+  <si>
+    <t>MIN_AGE_TO_RETIRE</t>
+  </si>
+  <si>
+    <t>DEFAULT_AGE_TO_RETIRE</t>
+  </si>
+  <si>
+    <t>MIN_AGE_FORMAL_SOCARE</t>
+  </si>
+  <si>
+    <t>MIN_AGE_FLEXIBLE_LABOUR_SUPPLY</t>
+  </si>
+  <si>
+    <t>MAX_AGE_FLEXIBLE_LABOUR_SUPPLY</t>
+  </si>
+  <si>
+    <t>SHARE_OF_WEALTH_TO_ANNUITISE_AT_RETIREMENT</t>
+  </si>
+  <si>
+    <t>ANNUITY_RATE_OF_RETURN</t>
+  </si>
+  <si>
+    <t>MIN_HOURS_FULL_TIME_EMPLOYED</t>
+  </si>
+  <si>
+    <t>MIN_HOURLY_WAGE_RATE</t>
+  </si>
+  <si>
+    <t>MAX_HOURLY_WAGE_RATE</t>
+  </si>
+  <si>
+    <t>MAX_HOURS_WEEKLY_FORMAL_CARE</t>
+  </si>
+  <si>
+    <t>MAX_HOURS_WEEKLY_INFORMAL_CARE</t>
+  </si>
+  <si>
+    <t>CHILDCARE_COST_EARNINGS_CAP</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -72,14 +127,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -92,9 +156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -102,44 +166,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -169,12 +233,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -204,7 +268,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -213,175 +277,200 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1328125" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -389,7 +478,160 @@
         <v>70</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now, all the country-specific parameters are set using the appropriate input country folder; all the necessary country-specific parameters are overwritten using the parameters.xlsx; column numbers parameters are loaded from columns_number_parameters.xlsx
</commit_message>
<xml_diff>
--- a/input/EL/parameters.xlsx
+++ b/input/EL/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9798C423-3424-C748-BB9F-B8CAF277D90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBC364F-5AF7-3146-8CF5-1F7FEE9A371B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="12560" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>KEY</t>
   </si>
@@ -92,19 +92,84 @@
   </si>
   <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>TAXDB_REGIMES</t>
+  </si>
+  <si>
+    <t>MIN_START_YEAR</t>
+  </si>
+  <si>
+    <t>MAX_START_YEAR</t>
+  </si>
+  <si>
+    <t>MIN_START_YEAR_TRAINING</t>
+  </si>
+  <si>
+    <t>MAX_START_YEAR_TRAINING</t>
+  </si>
+  <si>
+    <t>MIN_CAPITAL_INCOME_PER_MONTH</t>
+  </si>
+  <si>
+    <t>MAX_CAPITAL_INCOME_PER_MONTH</t>
+  </si>
+  <si>
+    <t>MIN_PERSONAL_PENSION_PER_MONTH</t>
+  </si>
+  <si>
+    <t>MAX_PERSONAL_PENSION_PER_MONTH</t>
+  </si>
+  <si>
+    <t>MAX_CHILD_AGE_FOR_FORMAL_CARE</t>
+  </si>
+  <si>
+    <t>MIN_AGE_MATERNITY</t>
+  </si>
+  <si>
+    <t>MAX_AGE_MATERNITY</t>
+  </si>
+  <si>
+    <t>BASE_PRICE_YEAR</t>
+  </si>
+  <si>
+    <t>PROB_NEWBORN_IS_MALE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFC77DBB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -138,6 +203,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,19 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -470,7 +539,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -478,7 +547,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -486,7 +555,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -494,7 +563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -502,7 +571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -510,7 +579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -518,7 +587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -526,7 +595,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -534,7 +603,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -542,7 +611,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -550,7 +619,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -558,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -566,7 +635,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -574,7 +643,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -582,7 +651,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -590,7 +659,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -598,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -606,7 +675,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -614,7 +683,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -622,13 +691,189 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>0.5</v>
       </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="7">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="7">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="6">
+        <v>44</v>
+      </c>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="6">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added additional country-specific parameters
Parameters are added to parameters.xlsx, they are applied in KeyFunctionHU2.java
also, fixed a typo in "MultiKey[HU]"
</commit_message>
<xml_diff>
--- a/input/EL/parameters.xlsx
+++ b/input/EL/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDFF257-DD58-824A-A7C1-5D7D557CCDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636346D8-D5F5-C64E-9DEF-7FC9651DE4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{FFF6265E-67A3-EB43-9D54-F28C7C01369A}"/>
+    <workbookView xWindow="12380" yWindow="6400" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{FFF6265E-67A3-EB43-9D54-F28C7C01369A}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
   <si>
     <t>KEY</t>
   </si>
@@ -271,6 +271,30 @@
   </si>
   <si>
     <t>Country-specific savings rate</t>
+  </si>
+  <si>
+    <t>KEY_FUNCTION_HU2_HI_INCOME</t>
+  </si>
+  <si>
+    <t>KEY_FUNCTION_HU2_LO_INCOME</t>
+  </si>
+  <si>
+    <t>KEY_FUNCTION_HU2_MID_AGE</t>
+  </si>
+  <si>
+    <t>KEY_FUNCTION_HU2_INCOME_REF_YEAR</t>
+  </si>
+  <si>
+    <t>67th percentile observed in the EM data for 2018</t>
+  </si>
+  <si>
+    <t>33rd percentile observed in the EM data for 2018</t>
+  </si>
+  <si>
+    <t>mid age of EM income data used in KeyFunctionHU2</t>
+  </si>
+  <si>
+    <t>year of EM income data used in KeyFunctionHU2</t>
   </si>
 </sst>
 </file>
@@ -335,16 +359,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374841C3-B837-9C4F-8C3E-3E56746FE108}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A37" sqref="A1:B37"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,170 +724,170 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
         <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="b">
+      <c r="B5" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15">
         <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19">
         <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20">
         <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21">
         <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22">
         <v>0.5</v>
       </c>
     </row>
@@ -980,11 +1004,43 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="A37" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37">
         <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="8">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="8">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
@@ -994,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27C737F-9315-9B4B-879C-C34F627BA824}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,6 +1363,38 @@
         <v>77</v>
       </c>
     </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>